<commit_message>
sae avancement vues et triggers
</commit_message>
<xml_diff>
--- a/Stage/Modèle de Carnet de bord.xlsx
+++ b/Stage/Modèle de Carnet de bord.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t xml:space="preserve">Date de l'offre</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Protection de l'environnement, spécialisation dans la magie et l'agriculture, vise la place de leader dans le marché de la transformation végétale</t>
   </si>
   <si>
-    <t xml:space="preserve">3 - Candidature soumise</t>
+    <t xml:space="preserve">5 - Refus</t>
   </si>
   <si>
     <t xml:space="preserve">Annonce web</t>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Machine learning, collecte de données, améliorer les capacités de langage naturel de la plate-forme ServiceNow, Données structurées (évolution de l’état du flux de travail, tables de base de données).Implémentez des interfaces Web à l’aide de frameworks JavaScript tels que React, Angular et CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 - Attente de réponse</t>
   </si>
   <si>
     <t xml:space="preserve">MONTREAL, dorval</t>
@@ -156,6 +159,9 @@
     <t xml:space="preserve">Stage Data Science Développement de Modèles de Data Science - IA Générative H/F</t>
   </si>
   <si>
+    <t xml:space="preserve">3 - Candidature soumise</t>
+  </si>
+  <si>
     <t xml:space="preserve">Astek, Paris 75</t>
   </si>
   <si>
@@ -165,35 +171,7 @@
     <t xml:space="preserve">Stage - - Stage de Fin d'Études - Ingénieur Innovation en Informatique Sciences des Données Ref-Bia-45 Paris France H/F</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">entreprise « green », big data, données médicales,graphe, traitement et </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">confidentialité </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">de données. Mission d’harmonisation des données médicales. Astek est un acteur mondial de l'ingénierie et du conseil en technologie. forte culture d'entrepreneuriat et d'innovation, accompagnement et la montée en compétence de ses 10.000 collaborateurs</t>
-    </r>
+    <t xml:space="preserve">entreprise « green », big data, données médicales,graphe, traitement et confidentialité de données. Mission d’harmonisation des données médicales. Astek est un acteur mondial de l'ingénierie et du conseil en technologie. forte culture d'entrepreneuriat et d'innovation, accompagnement et la montée en compétence de ses 10.000 collaborateurs</t>
   </si>
   <si>
     <t xml:space="preserve">Deepki, Paris 75011</t>
@@ -234,6 +212,15 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">entreprise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stagiaire 2Nde Opinion Tarification IARD H/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> réaliser une modélisation de la prime pure d'une garantie Auto,  comparer les résultats avec les modèles en production, tirer des conclusions permettant d'améliorer le processus global. Maitrise de Python et R demandé</t>
+  </si>
+  <si>
     <t xml:space="preserve">Origine Offre</t>
   </si>
   <si>
@@ -246,13 +233,7 @@
     <t xml:space="preserve">IUT à l'international</t>
   </si>
   <si>
-    <t xml:space="preserve">4 - Attente de réponse</t>
-  </si>
-  <si>
     <t xml:space="preserve">Candidature spontanée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 - Refus</t>
   </si>
   <si>
     <t xml:space="preserve">5 - Acceptation</t>
@@ -266,7 +247,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -310,12 +291,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -596,8 +571,8 @@
   </sheetPr>
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -658,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="104.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="111.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>45608</v>
       </c>
@@ -686,22 +661,22 @@
         <v>45608</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="104.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,39 +690,39 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="true" ht="138.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>45610</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,22 +730,22 @@
         <v>45608</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,11 +759,11 @@
         <v>14</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" s="6"/>
     </row>
@@ -797,22 +772,22 @@
         <v>45594</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="true" ht="144.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,32 +795,46 @@
         <v>45577</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" s="2" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
@@ -1736,7 +1725,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1751,10 +1740,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,18 +1756,18 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,20 +1775,20 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>